<commit_message>
add queries for combined rules and fill predictions for task 3 based on these rules
</commit_message>
<xml_diff>
--- a/Assignment2/BMKG_Assignment_2_predictions.xlsx
+++ b/Assignment2/BMKG_Assignment_2_predictions.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kody.moodley\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elena\Desktop\Master\Year1\Courses\BMKG\Assignments\BMKG2020\Assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DCD0F3-9E08-4695-9AE7-413C8C809C8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380"/>
+    <workbookView xWindow="8940" yWindow="3015" windowWidth="12840" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Task 3" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="20">
   <si>
     <t>Subject</t>
   </si>
@@ -49,13 +50,49 @@
   </si>
   <si>
     <t>Predicate 5: spouse - &lt;http://www.wikidata.org/prop/direct/P26&gt;</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q12702</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q4381482</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q333281</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q50025511</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q60749598</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q60749569</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q70045</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q64419436</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q12310272</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q261120</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q64416112</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q14646844</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +104,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -101,21 +146,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -124,19 +174,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -413,109 +463,157 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="46.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="46.85546875" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="46.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-    </row>
-    <row r="38" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -526,20 +624,30 @@
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="A49:C49"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B15" r:id="rId1" xr:uid="{D1E17ABD-729C-4982-9A01-97DCBB8FD73F}"/>
+    <hyperlink ref="A27" r:id="rId2" xr:uid="{D27BA660-6447-43D2-A0DE-D88B7E29E101}"/>
+    <hyperlink ref="B27" r:id="rId3" xr:uid="{5D77F38D-26C5-4200-AF84-8D8264C85E2D}"/>
+    <hyperlink ref="A51" r:id="rId4" xr:uid="{65674C80-0993-4E9A-BEF4-9A31C03EEE33}"/>
+    <hyperlink ref="B51" r:id="rId5" xr:uid="{D1A65650-1F99-46AA-9F61-ED00667C7932}"/>
+    <hyperlink ref="A52" r:id="rId6" xr:uid="{FAD55C50-E494-45D6-AE40-39A28B65A7BD}"/>
+    <hyperlink ref="A53" r:id="rId7" xr:uid="{BE5E58CF-B095-4AB3-A17D-A6D8311F6C51}"/>
+    <hyperlink ref="B54" r:id="rId8" xr:uid="{31C7E9F5-A4D8-48DF-9D7A-7F5E59D0E461}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.28515625" customWidth="1"/>
     <col min="2" max="2" width="47.85546875" customWidth="1"/>
@@ -547,242 +655,242 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C50" s="4" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add confidence scored for rules in excel sheet
</commit_message>
<xml_diff>
--- a/Assignment2/BMKG_Assignment_2_predictions.xlsx
+++ b/Assignment2/BMKG_Assignment_2_predictions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elena\Desktop\Master\Year1\Courses\BMKG\Assignments\BMKG2020\Assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DCD0F3-9E08-4695-9AE7-413C8C809C8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642AC409-D656-43B3-B532-F96436BDDA26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8940" yWindow="3015" windowWidth="12840" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="21">
   <si>
     <t>Subject</t>
   </si>
@@ -86,13 +86,16 @@
   </si>
   <si>
     <t>http://www.wikidata.org/entity/Q14646844</t>
+  </si>
+  <si>
+    <t>88.8%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,14 +107,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -146,9 +141,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -180,12 +174,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -466,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,6 +514,9 @@
       <c r="B15" s="11" t="s">
         <v>9</v>
       </c>
+      <c r="C15" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -547,6 +543,9 @@
       <c r="B27" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
@@ -591,6 +590,9 @@
       <c r="B51" s="11" t="s">
         <v>17</v>
       </c>
+      <c r="C51" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
@@ -599,6 +601,9 @@
       <c r="B52" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="C52" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
@@ -607,6 +612,9 @@
       <c r="B53" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="C53" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
@@ -614,6 +622,9 @@
       </c>
       <c r="B54" s="11" t="s">
         <v>19</v>
+      </c>
+      <c r="C54" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -624,18 +635,8 @@
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="A49:C49"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B15" r:id="rId1" xr:uid="{D1E17ABD-729C-4982-9A01-97DCBB8FD73F}"/>
-    <hyperlink ref="A27" r:id="rId2" xr:uid="{D27BA660-6447-43D2-A0DE-D88B7E29E101}"/>
-    <hyperlink ref="B27" r:id="rId3" xr:uid="{5D77F38D-26C5-4200-AF84-8D8264C85E2D}"/>
-    <hyperlink ref="A51" r:id="rId4" xr:uid="{65674C80-0993-4E9A-BEF4-9A31C03EEE33}"/>
-    <hyperlink ref="B51" r:id="rId5" xr:uid="{D1A65650-1F99-46AA-9F61-ED00667C7932}"/>
-    <hyperlink ref="A52" r:id="rId6" xr:uid="{FAD55C50-E494-45D6-AE40-39A28B65A7BD}"/>
-    <hyperlink ref="A53" r:id="rId7" xr:uid="{BE5E58CF-B095-4AB3-A17D-A6D8311F6C51}"/>
-    <hyperlink ref="B54" r:id="rId8" xr:uid="{31C7E9F5-A4D8-48DF-9D7A-7F5E59D0E461}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>